<commit_message>
1.delete insert.sql files  2.modified database designed excel file
</commit_message>
<xml_diff>
--- a/db/dev/表结构设计.xlsx
+++ b/db/dev/表结构设计.xlsx
@@ -21,7 +21,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="90" uniqueCount="58">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="66">
   <si>
     <t>id</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -252,6 +252,38 @@
   </si>
   <si>
     <t>taskId</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>部门表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户-部门表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>用户-项目表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>项目评论表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务表</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>任务评论表</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -601,6 +633,190 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B11"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A12" sqref="A12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>58</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>2</v>
+      </c>
+      <c r="B3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>4</v>
+      </c>
+      <c r="B4" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>6</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>8</v>
+      </c>
+      <c r="B6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B7" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A8" t="s">
+        <v>12</v>
+      </c>
+      <c r="B8" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>14</v>
+      </c>
+      <c r="B9" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A11" t="s">
+        <v>16</v>
+      </c>
+      <c r="B11" t="s">
+        <v>17</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A5" sqref="A5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>59</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>0</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>33</v>
+      </c>
+      <c r="B3" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B4" t="s">
+        <v>32</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A6" sqref="A6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
+  <cols>
+    <col min="1" max="2" width="20.625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A1" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A2" t="s">
+        <v>50</v>
+      </c>
+      <c r="B2" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>52</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="1" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B10"/>
   <sheetViews>
     <sheetView workbookViewId="0">
@@ -611,74 +827,79 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+        <v>61</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>7</v>
+        <v>21</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
-        <v>8</v>
+        <v>28</v>
       </c>
       <c r="B5" t="s">
-        <v>9</v>
+        <v>38</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>34</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>35</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>12</v>
+        <v>36</v>
       </c>
       <c r="B7" t="s">
-        <v>13</v>
+        <v>37</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>14</v>
+        <v>39</v>
       </c>
       <c r="B8" t="s">
-        <v>15</v>
+        <v>40</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A9" t="s">
+        <v>22</v>
+      </c>
+      <c r="B9" t="s">
+        <v>23</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A10" t="s">
-        <v>16</v>
+        <v>14</v>
       </c>
       <c r="B10" t="s">
-        <v>17</v>
+        <v>15</v>
       </c>
     </row>
   </sheetData>
@@ -688,38 +909,48 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B3"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A4" sqref="A4"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+        <v>62</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>33</v>
+        <v>24</v>
       </c>
       <c r="B2" t="s">
-        <v>30</v>
+        <v>25</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>31</v>
+        <v>26</v>
       </c>
       <c r="B3" t="s">
-        <v>32</v>
+        <v>27</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B4" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>49</v>
       </c>
     </row>
   </sheetData>
@@ -728,47 +959,69 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <cols>
-    <col min="1" max="2" width="20.625" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>50</v>
-      </c>
-      <c r="B1" t="s">
-        <v>51</v>
+        <v>63</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>26</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>27</v>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A3" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" t="s">
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>52</v>
+        <v>24</v>
+      </c>
+      <c r="B4" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
+        <v>14</v>
+      </c>
+      <c r="B6" t="s">
+        <v>55</v>
       </c>
     </row>
   </sheetData>
   <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B9"/>
   <sheetViews>
@@ -780,34 +1033,31 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+        <v>64</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>18</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>19</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B3" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>28</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>38</v>
+        <v>42</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
@@ -820,26 +1070,26 @@
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A6" t="s">
-        <v>36</v>
+        <v>45</v>
       </c>
       <c r="B6" t="s">
-        <v>37</v>
+        <v>44</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A7" t="s">
-        <v>39</v>
+        <v>22</v>
       </c>
       <c r="B7" t="s">
-        <v>40</v>
+        <v>43</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A8" t="s">
-        <v>22</v>
+        <v>36</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>46</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.15">
@@ -847,189 +1097,6 @@
         <v>14</v>
       </c>
       <c r="B9" t="s">
-        <v>15</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>24</v>
-      </c>
-      <c r="B1" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>26</v>
-      </c>
-      <c r="B2" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>28</v>
-      </c>
-      <c r="B3" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>49</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>47</v>
-      </c>
-      <c r="B2" t="s">
-        <v>48</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>24</v>
-      </c>
-      <c r="B3" t="s">
-        <v>53</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>26</v>
-      </c>
-      <c r="B4" t="s">
-        <v>54</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" t="s">
-        <v>55</v>
-      </c>
-    </row>
-  </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B8"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A9" sqref="A9"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr defaultColWidth="20.625" defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
-  <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A2" t="s">
-        <v>18</v>
-      </c>
-      <c r="B2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A3" t="s">
-        <v>20</v>
-      </c>
-      <c r="B3" t="s">
-        <v>42</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A4" t="s">
-        <v>34</v>
-      </c>
-      <c r="B4" t="s">
-        <v>35</v>
-      </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A5" t="s">
-        <v>45</v>
-      </c>
-      <c r="B5" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A6" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" t="s">
-        <v>43</v>
-      </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A7" t="s">
-        <v>36</v>
-      </c>
-      <c r="B7" t="s">
-        <v>46</v>
-      </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.15">
-      <c r="A8" t="s">
-        <v>14</v>
-      </c>
-      <c r="B8" t="s">
         <v>15</v>
       </c>
     </row>
@@ -1042,10 +1109,10 @@
 
 <file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:B5"/>
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A6" sqref="A6"/>
+      <selection activeCell="A7" sqref="A7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.5" x14ac:dyDescent="0.15"/>
@@ -1055,41 +1122,46 @@
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A1" t="s">
-        <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
+        <v>65</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A2" t="s">
-        <v>47</v>
+        <v>0</v>
       </c>
       <c r="B2" t="s">
-        <v>48</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A3" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
       <c r="B3" t="s">
-        <v>56</v>
+        <v>48</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A4" t="s">
-        <v>26</v>
+        <v>57</v>
       </c>
       <c r="B4" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.15">
       <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>54</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.15">
+      <c r="A6" t="s">
         <v>14</v>
       </c>
-      <c r="B5" t="s">
+      <c r="B6" t="s">
         <v>55</v>
       </c>
     </row>

</xml_diff>